<commit_message>
parameterised and more organised version of test_signup.py file. created helper file for signup too
</commit_message>
<xml_diff>
--- a/reports/test_signup_report.xlsx
+++ b/reports/test_signup_report.xlsx
@@ -45,8 +45,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00C6EFCE"/>
-        <bgColor rgb="00C6EFCE"/>
+        <fgColor rgb="00FFC7CE"/>
+        <bgColor rgb="00FFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,29 +536,29 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H2" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I2" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -585,29 +585,29 @@
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H3" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I3" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -624,7 +624,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Verify signup with full name required error.</t>
+          <t>Verify full name required error.</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -634,29 +634,29 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G4" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H4" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I4" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -673,7 +673,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>Verify signup with email required error.</t>
+          <t>Verify email required error.</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -683,29 +683,29 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G5" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H5" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I5" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -722,7 +722,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>Verify signup with password required error.</t>
+          <t>Verify password required error.</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -732,29 +732,29 @@
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G6" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H6" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I6" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -771,7 +771,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>Verify signup with confirm password required error.</t>
+          <t>Verify confirm password required error.</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
@@ -781,29 +781,29 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G7" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H7" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I7" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -820,7 +820,7 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>Verify signup with password mismatch error.</t>
+          <t>Verify password mismatch error.</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
@@ -830,29 +830,29 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G8" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H8" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I8" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>Verify signup with invalid email format.</t>
+          <t>Verify invalid email format error.</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
@@ -879,29 +879,29 @@
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G9" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H9" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I9" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -918,7 +918,7 @@
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>Verify signup with existing email.</t>
+          <t>Verify existing email error.</t>
         </is>
       </c>
       <c r="D10" s="3" t="inlineStr">
@@ -928,29 +928,29 @@
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G10" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H10" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I10" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -967,7 +967,7 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>Verify signup with public domain email warning.</t>
+          <t>Verify public domain email warning.</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
@@ -977,29 +977,29 @@
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G11" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H11" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I11" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>Verify signup with weak password warning.</t>
+          <t>Verify weak password warning.</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
@@ -1026,29 +1026,29 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G12" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H12" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I12" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1075,29 +1075,29 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G13" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H13" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I13" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1124,29 +1124,29 @@
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G14" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H14" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I14" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1173,29 +1173,29 @@
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H15" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I15" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1222,29 +1222,29 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G16" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H16" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I16" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1271,29 +1271,29 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G17" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H17" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I17" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>Verify full name can not start or end with special characters.</t>
+          <t>Verify full name cannot start or end with special characters.</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
@@ -1320,29 +1320,29 @@
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G18" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H18" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I18" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1369,29 +1369,29 @@
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G19" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H19" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I19" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1418,29 +1418,29 @@
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G20" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H20" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I20" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1467,29 +1467,29 @@
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G21" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H21" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I21" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1516,29 +1516,29 @@
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G22" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H22" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I22" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1565,29 +1565,29 @@
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G23" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H23" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
+          <t>Test failed - actual behavior did not match expected result</t>
         </is>
       </c>
       <c r="I23" s="4" t="inlineStr">
         <is>
-          <t>PASSED</t>
+          <t>FAILED</t>
         </is>
       </c>
     </row>
@@ -1614,29 +1614,29 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G24" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H24" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I24" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1663,29 +1663,29 @@
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G25" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H25" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I25" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1712,29 +1712,29 @@
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G26" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H26" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I26" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I26" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>Verify visibility of email verification page.</t>
+          <t>Verify email verification page visibility.</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
@@ -1761,29 +1761,29 @@
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G27" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H27" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I27" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>Verify visibility of OTP verification page heading.</t>
+          <t>Verify OTP verification page heading visibility.</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
@@ -1810,29 +1810,29 @@
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G28" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H28" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I28" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1849,7 +1849,7 @@
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>Verify visibility of mailbox image on verification page.</t>
+          <t>Verify mailbox image visibility on verification page.</t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
@@ -1859,29 +1859,29 @@
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G29" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H29" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I29" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1898,7 +1898,7 @@
       </c>
       <c r="C30" s="3" t="inlineStr">
         <is>
-          <t>Verify visibility of verification instructions on verification page.</t>
+          <t>Verify verification instructions visibility on verification page.</t>
         </is>
       </c>
       <c r="D30" s="3" t="inlineStr">
@@ -1908,29 +1908,29 @@
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G30" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H30" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I30" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I30" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="C31" s="3" t="inlineStr">
         <is>
-          <t>Verify visibility of OTP input box on verification page.</t>
+          <t>Verify OTP input box visibility on verification page.</t>
         </is>
       </c>
       <c r="D31" s="3" t="inlineStr">
@@ -1957,29 +1957,29 @@
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G31" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H31" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I31" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I31" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1996,7 +1996,7 @@
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>Verify visibility of input box title on verification page.</t>
+          <t>Verify input box title visibility on verification page.</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
@@ -2006,29 +2006,29 @@
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G32" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H32" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I32" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>Verify visibility of verify button on verification page.</t>
+          <t>Verify verify button visibility on verification page.</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
@@ -2055,29 +2055,29 @@
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G33" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H33" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I33" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="C34" s="3" t="inlineStr">
         <is>
-          <t>Verify visibility of resend OTP button on verification page.</t>
+          <t>Verify resend OTP countdown visibility on verification page.</t>
         </is>
       </c>
       <c r="D34" s="3" t="inlineStr">
@@ -2104,78 +2104,29 @@
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>Signup form data</t>
+          <t>Signup test data</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
+2. Perform required actions
+3. Verify expected behavior</t>
         </is>
       </c>
       <c r="G34" s="3" t="inlineStr">
         <is>
-          <t>Signup process should work as expected</t>
+          <t>Signup functionality should work as expected</t>
         </is>
       </c>
       <c r="H34" s="3" t="inlineStr">
         <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I34" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
-        </is>
-      </c>
-    </row>
-    <row r="35" ht="80" customHeight="1">
-      <c r="A35" s="2" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="B35" s="3" t="inlineStr">
-        <is>
-          <t>TC_034</t>
-        </is>
-      </c>
-      <c r="C35" s="3" t="inlineStr">
-        <is>
-          <t>Verify visibility of resend OTP countdown on verification page.</t>
-        </is>
-      </c>
-      <c r="D35" s="3" t="inlineStr">
-        <is>
-          <t>User is on the signup page</t>
-        </is>
-      </c>
-      <c r="E35" s="3" t="inlineStr">
-        <is>
-          <t>Signup form data</t>
-        </is>
-      </c>
-      <c r="F35" s="3" t="inlineStr">
-        <is>
-          <t>1. Navigate to signup page
-2. Fill required fields
-3. Submit form</t>
-        </is>
-      </c>
-      <c r="G35" s="3" t="inlineStr">
-        <is>
-          <t>Signup process should work as expected</t>
-        </is>
-      </c>
-      <c r="H35" s="3" t="inlineStr">
-        <is>
-          <t>Signup functionality verified</t>
-        </is>
-      </c>
-      <c r="I35" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I34" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>

</xml_diff>